<commit_message>
Fixed DQ6 seed location
</commit_message>
<xml_diff>
--- a/DQ6/DQ6_Data.xlsx
+++ b/DQ6/DQ6_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Paraz10\Documents\Projets\Dragon Quest 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paraz\Documents\Travail\ProjetsPerso\DQ_DS\DQ_DS_Data\DQ6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C68F12-12F1-4864-8EDC-F3BF27376060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF811029-D65A-420A-8202-6558453740DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Seed</t>
   </si>
   <si>
-    <t>02101564</t>
-  </si>
-  <si>
     <t>020DD52C</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>020BA3AC</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +451,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -463,41 +463,41 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the DQ4 functions to find the unique value of the console
</commit_message>
<xml_diff>
--- a/DQ6/DQ6_Data.xlsx
+++ b/DQ6/DQ6_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paraz\Documents\Travail\ProjetsPerso\DQ_DS\DQ_DS_Data\DQ6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Paraz10\Documents\Projets\DQ_4-5-6_DS_Data\DQ6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52F53C2-EB90-41B3-A3FB-0017D5BF1679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A229CD7-66CE-4E62-B68C-292767D6C05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Adress</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>020BA3AC</t>
+  </si>
+  <si>
+    <t>Other Informations</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Encounter Table</t>
+  </si>
+  <si>
+    <t>The encounter table that rules which monsters can be encountered</t>
+  </si>
+  <si>
+    <t>0212CBB4</t>
   </si>
 </sst>
 </file>
@@ -419,20 +434,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="25.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="6" width="60.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +463,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -466,7 +484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -483,7 +501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -498,6 +516,23 @@
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>